<commit_message>
Assignment2 submission with error graph images at various Learning rates
</commit_message>
<xml_diff>
--- a/Session2-Assignment/NN_Backpropagation_with_example.xlsx
+++ b/Session2-Assignment/NN_Backpropagation_with_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smruthi.r\Documents\Smruthi_Learning\END2\Session2-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F7FBEB-ACD1-41CD-9C49-370F193BAF87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E79E55-C35C-4F8C-B2B7-F4499E1415A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{B02C46A5-755B-4CE4-8937-6666101DAF8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{B02C46A5-755B-4CE4-8937-6666101DAF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="NN-ɳ=0.1" sheetId="2" r:id="rId1"/>
@@ -388,7 +388,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -467,7 +467,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8528,15 +8528,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>28086</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>167054</xdr:rowOff>
+      <xdr:colOff>28085</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>36634</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>326048</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>232019</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>174869</xdr:rowOff>
+      <xdr:rowOff>85481</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10723,15 +10723,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>28086</xdr:colOff>
+      <xdr:colOff>28085</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>167054</xdr:rowOff>
+      <xdr:rowOff>24423</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>326048</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>174869</xdr:rowOff>
+      <xdr:colOff>610576</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12210</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15110,16 +15110,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>28086</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>167054</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>357798</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>326048</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>174869</xdr:rowOff>
+      <xdr:colOff>464039</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17306,13 +17306,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>28086</xdr:colOff>
+      <xdr:colOff>28085</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>167054</xdr:rowOff>
+      <xdr:rowOff>24423</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>326048</xdr:colOff>
+      <xdr:colOff>561731</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>174869</xdr:rowOff>
     </xdr:to>
@@ -19503,13 +19503,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>28086</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>167054</xdr:rowOff>
+      <xdr:rowOff>61058</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>326048</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>174869</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>24423</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19838,7 +19838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CFB711-D56C-4B61-9D06-0524BB0DB0BE}">
   <dimension ref="A2:AE84"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -20388,7 +20388,7 @@
         <v>0.1</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:H84" si="2">E34-$G$31*X34</f>
+        <f t="shared" ref="E35:H80" si="2">E34-$G$31*X34</f>
         <v>0.14996396683792318</v>
       </c>
       <c r="F35">
@@ -20404,7 +20404,7 @@
         <v>0.29991331885621669</v>
       </c>
       <c r="I35">
-        <f t="shared" ref="I35:I84" si="3">E35*C35+F35*D35</f>
+        <f t="shared" ref="I35:I71" si="3">E35*C35+F35*D35</f>
         <v>2.7490991709480796E-2</v>
       </c>
       <c r="J35" s="3">
@@ -20412,7 +20412,7 @@
         <v>0.50687231511749375</v>
       </c>
       <c r="K35">
-        <f t="shared" ref="K35:K84" si="5">G35*C35+H35*D35</f>
+        <f t="shared" ref="K35:K71" si="5">G35*C35+H35*D35</f>
         <v>4.2489164857027084E-2</v>
       </c>
       <c r="L35" s="7">
@@ -20420,7 +20420,7 @@
         <v>0.51062069344172678</v>
       </c>
       <c r="M35">
-        <f t="shared" ref="M35:P84" si="7">M34-$G$31*AB34</f>
+        <f t="shared" ref="M35:P80" si="7">M34-$G$31*AB34</f>
         <v>0.38557869053883581</v>
       </c>
       <c r="N35">
@@ -20436,7 +20436,7 @@
         <v>0.55853699155539305</v>
       </c>
       <c r="Q35" s="4">
-        <f t="shared" ref="Q35:Q84" si="8">M35*J35+N35*L35</f>
+        <f t="shared" ref="Q35:Q71" si="8">M35*J35+N35*L35</f>
         <v>0.41780019547766128</v>
       </c>
       <c r="R35" s="5">
@@ -20444,7 +20444,7 @@
         <v>0.60295673631866042</v>
       </c>
       <c r="S35" s="4">
-        <f t="shared" ref="S35:S84" si="10">O35*J35+P35*L35</f>
+        <f t="shared" ref="S35:S71" si="10">O35*J35+P35*L35</f>
         <v>0.54293210043063311</v>
       </c>
       <c r="T35" s="5">
@@ -20452,11 +20452,11 @@
         <v>0.63249423502317081</v>
       </c>
       <c r="U35" s="5">
-        <f t="shared" ref="U35:U84" si="12">1/2*(A35-R35)^2</f>
+        <f t="shared" ref="U35:U71" si="12">1/2*(A35-R35)^2</f>
         <v>0.17579884557283867</v>
       </c>
       <c r="V35" s="5">
-        <f t="shared" ref="V35:V84" si="13">1/2*(B35-T35)^2</f>
+        <f t="shared" ref="V35:V71" si="13">1/2*(B35-T35)^2</f>
         <v>6.3905185995833905E-2</v>
       </c>
       <c r="W35" s="5">
@@ -20464,35 +20464,35 @@
         <v>0.23970403156867259</v>
       </c>
       <c r="X35" s="4">
-        <f t="shared" ref="X35:X84" si="15">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*C35</f>
+        <f t="shared" ref="X35:X71" si="15">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*C35</f>
         <v>1.5596893764313439E-4</v>
       </c>
       <c r="Y35" s="4">
-        <f t="shared" ref="Y35:Y84" si="16">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*D35</f>
+        <f t="shared" ref="Y35:Y71" si="16">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*D35</f>
         <v>3.1193787528626879E-4</v>
       </c>
       <c r="Z35" s="4">
-        <f t="shared" ref="Z35:Z84" si="17">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*C35</f>
+        <f t="shared" ref="Z35:Z71" si="17">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*C35</f>
         <v>1.9244047267639547E-4</v>
       </c>
       <c r="AA35" s="4">
-        <f t="shared" ref="AA35:AA84" si="18">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*D35</f>
+        <f t="shared" ref="AA35:AA71" si="18">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*D35</f>
         <v>3.8488094535279094E-4</v>
       </c>
       <c r="AB35" s="4">
-        <f t="shared" ref="AB35:AB84" si="19">(R35-A35)*R35*(1-R35)*J35</f>
+        <f t="shared" ref="AB35:AB71" si="19">(R35-A35)*R35*(1-R35)*J35</f>
         <v>7.195244596077148E-2</v>
       </c>
       <c r="AC35" s="4">
-        <f t="shared" ref="AC35:AC84" si="20">(R35-A35)*R35*(1-R35)*L35</f>
+        <f t="shared" ref="AC35:AC71" si="20">(R35-A35)*R35*(1-R35)*L35</f>
         <v>7.2484542468651145E-2</v>
       </c>
       <c r="AD35">
-        <f t="shared" ref="AD35:AD84" si="21">(T35-B35)*T35*(1-T35)*J35</f>
+        <f t="shared" ref="AD35:AD71" si="21">(T35-B35)*T35*(1-T35)*J35</f>
         <v>-4.2121356413822648E-2</v>
       </c>
       <c r="AE35">
-        <f t="shared" ref="AE35:AE84" si="22">(T35-B35)*T35*(1-T35)*L35</f>
+        <f t="shared" ref="AE35:AE71" si="22">(T35-B35)*T35*(1-T35)*L35</f>
         <v>-4.2432848627265533E-2</v>
       </c>
     </row>
@@ -26064,8 +26064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7164657C-5317-42AD-B9D5-E5FDAA550C43}">
   <dimension ref="A2:AE84"/>
   <sheetViews>
-    <sheetView topLeftCell="C9" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="AB13" sqref="AB13"/>
+    <sheetView topLeftCell="F3" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="AB22" sqref="AB22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26614,7 +26614,7 @@
         <v>0.1</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:H84" si="2">E34-$G$31*X34</f>
+        <f t="shared" ref="E35:H80" si="2">E34-$G$31*X34</f>
         <v>0.14993116078010463</v>
       </c>
       <c r="F35">
@@ -26630,7 +26630,7 @@
         <v>0.29983310968176186</v>
       </c>
       <c r="I35">
-        <f t="shared" ref="I35:I84" si="3">E35*C35+F35*D35</f>
+        <f t="shared" ref="I35:I71" si="3">E35*C35+F35*D35</f>
         <v>2.7482790195026162E-2</v>
       </c>
       <c r="J35" s="3">
@@ -26638,7 +26638,7 @@
         <v>0.50687026512611166</v>
       </c>
       <c r="K35">
-        <f t="shared" ref="K35:K84" si="5">G35*C35+H35*D35</f>
+        <f t="shared" ref="K35:K71" si="5">G35*C35+H35*D35</f>
         <v>4.2479138710220236E-2</v>
       </c>
       <c r="L35" s="7">
@@ -26646,7 +26646,7 @@
         <v>0.51061818803569892</v>
       </c>
       <c r="M35">
-        <f t="shared" ref="M35:P84" si="7">M34-$G$31*AB34</f>
+        <f t="shared" ref="M35:P80" si="7">M34-$G$31*AB34</f>
         <v>0.37117812871672973</v>
       </c>
       <c r="N35">
@@ -26662,7 +26662,7 @@
         <v>0.56704028580862431</v>
       </c>
       <c r="Q35" s="4">
-        <f t="shared" ref="Q35:Q84" si="8">M35*J35+N35*L35</f>
+        <f t="shared" ref="Q35:Q71" si="8">M35*J35+N35*L35</f>
         <v>0.40309152936704296</v>
       </c>
       <c r="R35" s="5">
@@ -26670,7 +26670,7 @@
         <v>0.5994302061245802</v>
       </c>
       <c r="S35" s="4">
-        <f t="shared" ref="S35:S84" si="10">O35*J35+P35*L35</f>
+        <f t="shared" ref="S35:S71" si="10">O35*J35+P35*L35</f>
         <v>0.55155002202717229</v>
       </c>
       <c r="T35" s="5">
@@ -26678,11 +26678,11 @@
         <v>0.63449513314275852</v>
       </c>
       <c r="U35" s="5">
-        <f t="shared" ref="U35:U84" si="12">1/2*(A35-R35)^2</f>
+        <f t="shared" ref="U35:U71" si="12">1/2*(A35-R35)^2</f>
         <v>0.17371398394603255</v>
       </c>
       <c r="V35" s="5">
-        <f t="shared" ref="V35:V84" si="13">1/2*(B35-T35)^2</f>
+        <f t="shared" ref="V35:V71" si="13">1/2*(B35-T35)^2</f>
         <v>6.3191855179592499E-2</v>
       </c>
       <c r="W35" s="5">
@@ -26690,35 +26690,35 @@
         <v>0.23690583912562505</v>
       </c>
       <c r="X35" s="4">
-        <f t="shared" ref="X35:X84" si="15">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*C35</f>
+        <f t="shared" ref="X35:X71" si="15">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*C35</f>
         <v>1.2392146184868918E-4</v>
       </c>
       <c r="Y35" s="4">
-        <f t="shared" ref="Y35:Y84" si="16">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*D35</f>
+        <f t="shared" ref="Y35:Y71" si="16">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*D35</f>
         <v>2.4784292369737837E-4</v>
       </c>
       <c r="Z35" s="4">
-        <f t="shared" ref="Z35:Z84" si="17">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*C35</f>
+        <f t="shared" ref="Z35:Z71" si="17">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*C35</f>
         <v>1.6029447221242507E-4</v>
       </c>
       <c r="AA35" s="4">
-        <f t="shared" ref="AA35:AA84" si="18">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*D35</f>
+        <f t="shared" ref="AA35:AA71" si="18">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*D35</f>
         <v>3.2058894442485013E-4</v>
       </c>
       <c r="AB35" s="4">
-        <f t="shared" ref="AB35:AB84" si="19">(R35-A35)*R35*(1-R35)*J35</f>
+        <f t="shared" ref="AB35:AB71" si="19">(R35-A35)*R35*(1-R35)*J35</f>
         <v>7.1737464618933308E-2</v>
       </c>
       <c r="AC35" s="4">
-        <f t="shared" ref="AC35:AC84" si="20">(R35-A35)*R35*(1-R35)*L35</f>
+        <f t="shared" ref="AC35:AC71" si="20">(R35-A35)*R35*(1-R35)*L35</f>
         <v>7.2267909006027337E-2</v>
       </c>
       <c r="AD35">
-        <f t="shared" ref="AD35:AD84" si="21">(T35-B35)*T35*(1-T35)*J35</f>
+        <f t="shared" ref="AD35:AD71" si="21">(T35-B35)*T35*(1-T35)*J35</f>
         <v>-4.1789177618459211E-2</v>
       </c>
       <c r="AE35">
-        <f t="shared" ref="AE35:AE84" si="22">(T35-B35)*T35*(1-T35)*L35</f>
+        <f t="shared" ref="AE35:AE71" si="22">(T35-B35)*T35*(1-T35)*L35</f>
         <v>-4.2098177034966835E-2</v>
       </c>
     </row>
@@ -32290,7 +32290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93550F1-B463-4C6D-A702-C79FD9358462}">
   <dimension ref="A2:AE84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView topLeftCell="E2" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -32840,111 +32840,111 @@
         <v>0.1</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:E84" si="2">E34-$G$31*X34</f>
+        <f t="shared" ref="E35:E71" si="2">E34-$G$31*X34</f>
         <v>0.14985196558306668</v>
       </c>
       <c r="F35">
-        <f t="shared" ref="F35:F84" si="3">F34-$G$31*Y34</f>
+        <f t="shared" ref="F35:F72" si="3">F34-$G$31*Y34</f>
         <v>0.19970393116613333</v>
       </c>
       <c r="G35">
-        <f t="shared" ref="G35:G84" si="4">G34-$G$31*Z34</f>
+        <f t="shared" ref="G35:G72" si="4">G34-$G$31*Z34</f>
         <v>0.24981552599600967</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H35:H84" si="5">H34-$G$31*AA34</f>
+        <f t="shared" ref="H35:H72" si="5">H34-$G$31*AA34</f>
         <v>0.29963105199201934</v>
       </c>
       <c r="I35">
-        <f t="shared" ref="I35:I84" si="6">E35*C35+F35*D35</f>
+        <f t="shared" ref="I35:I71" si="6">E35*C35+F35*D35</f>
         <v>2.7462991395766669E-2</v>
       </c>
       <c r="J35" s="3">
-        <f t="shared" ref="J35:J84" si="7">1/(1+EXP(-I35))</f>
+        <f t="shared" ref="J35:J80" si="7">1/(1+EXP(-I35))</f>
         <v>0.50686531636013787</v>
       </c>
       <c r="K35">
-        <f t="shared" ref="K35:K84" si="8">G35*C35+H35*D35</f>
+        <f t="shared" ref="K35:K71" si="8">G35*C35+H35*D35</f>
         <v>4.2453881499002422E-2</v>
       </c>
       <c r="L35" s="7">
-        <f t="shared" ref="L35:L84" si="9">1/(1+EXP(-K35))</f>
+        <f t="shared" ref="L35:L80" si="9">1/(1+EXP(-K35))</f>
         <v>0.51061187657884965</v>
       </c>
       <c r="M35">
-        <f t="shared" ref="M35:M84" si="10">M34-$G$31*AB34</f>
+        <f t="shared" ref="M35:M71" si="10">M34-$G$31*AB34</f>
         <v>0.32810895116557248</v>
       </c>
       <c r="N35">
-        <f t="shared" ref="N35:N84" si="11">N34-$G$31*AC34</f>
+        <f t="shared" ref="N35:N72" si="11">N34-$G$31*AC34</f>
         <v>0.37757732389332388</v>
       </c>
       <c r="O35">
-        <f t="shared" ref="O35:O84" si="12">O34-$G$31*AD34</f>
+        <f t="shared" ref="O35:O72" si="12">O34-$G$31*AD34</f>
         <v>0.542037428831741</v>
       </c>
       <c r="P35">
-        <f t="shared" ref="P35:P84" si="13">P34-$G$31*AE34</f>
+        <f t="shared" ref="P35:P72" si="13">P34-$G$31*AE34</f>
         <v>0.59234829178874815</v>
       </c>
       <c r="Q35" s="4">
-        <f t="shared" ref="Q35:Q84" si="14">M35*J35+N35*L35</f>
+        <f t="shared" ref="Q35:Q71" si="14">M35*J35+N35*L35</f>
         <v>0.35910251323992115</v>
       </c>
       <c r="R35" s="5">
-        <f t="shared" ref="R35:R84" si="15">1/(1+EXP(-Q35))</f>
+        <f t="shared" ref="R35:R80" si="15">1/(1+EXP(-Q35))</f>
         <v>0.58882316047387184</v>
       </c>
       <c r="S35" s="4">
-        <f t="shared" ref="S35:S84" si="16">O35*J35+P35*L35</f>
+        <f t="shared" ref="S35:S71" si="16">O35*J35+P35*L35</f>
         <v>0.57720004570236483</v>
       </c>
       <c r="T35" s="5">
-        <f t="shared" ref="T35:T84" si="17">1/(1+EXP(-S35))</f>
+        <f t="shared" ref="T35:T80" si="17">1/(1+EXP(-S35))</f>
         <v>0.64042288273336123</v>
       </c>
       <c r="U35" s="5">
-        <f t="shared" ref="U35:U84" si="18">1/2*(A35-R35)^2</f>
+        <f t="shared" ref="U35:U71" si="18">1/2*(A35-R35)^2</f>
         <v>0.16751812555048079</v>
       </c>
       <c r="V35" s="5">
-        <f t="shared" ref="V35:V84" si="19">1/2*(B35-T35)^2</f>
+        <f t="shared" ref="V35:V71" si="19">1/2*(B35-T35)^2</f>
         <v>6.1102080458226654E-2</v>
       </c>
       <c r="W35" s="5">
-        <f t="shared" ref="W35:W84" si="20">U35+V35</f>
+        <f t="shared" ref="W35:W71" si="20">U35+V35</f>
         <v>0.22862020600870744</v>
       </c>
       <c r="X35" s="4">
-        <f t="shared" ref="X35:X84" si="21">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*C35</f>
+        <f t="shared" ref="X35:X71" si="21">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*C35</f>
         <v>2.9323069624365552E-5</v>
       </c>
       <c r="Y35" s="4">
-        <f t="shared" ref="Y35:Y84" si="22">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*D35</f>
+        <f t="shared" ref="Y35:Y71" si="22">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*D35</f>
         <v>5.8646139248731104E-5</v>
       </c>
       <c r="Z35" s="4">
-        <f t="shared" ref="Z35:Z84" si="23">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*C35</f>
+        <f t="shared" ref="Z35:Z71" si="23">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*C35</f>
         <v>6.5328838952553596E-5</v>
       </c>
       <c r="AA35" s="4">
-        <f t="shared" ref="AA35:AA84" si="24">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*D35</f>
+        <f t="shared" ref="AA35:AA71" si="24">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*D35</f>
         <v>1.3065767790510719E-4</v>
       </c>
       <c r="AB35" s="4">
-        <f t="shared" ref="AB35:AB84" si="25">(R35-A35)*R35*(1-R35)*J35</f>
+        <f t="shared" ref="AB35:AB71" si="25">(R35-A35)*R35*(1-R35)*J35</f>
         <v>7.1031666302848406E-2</v>
       </c>
       <c r="AC35" s="4">
-        <f t="shared" ref="AC35:AC84" si="26">(R35-A35)*R35*(1-R35)*L35</f>
+        <f t="shared" ref="AC35:AC71" si="26">(R35-A35)*R35*(1-R35)*L35</f>
         <v>7.1556706005999005E-2</v>
       </c>
       <c r="AD35">
-        <f t="shared" ref="AD35:AD84" si="27">(T35-B35)*T35*(1-T35)*J35</f>
+        <f t="shared" ref="AD35:AD71" si="27">(T35-B35)*T35*(1-T35)*J35</f>
         <v>-4.0803222041132202E-2</v>
       </c>
       <c r="AE35">
-        <f t="shared" ref="AE35:AE84" si="28">(T35-B35)*T35*(1-T35)*L35</f>
+        <f t="shared" ref="AE35:AE71" si="28">(T35-B35)*T35*(1-T35)*L35</f>
         <v>-4.110482430816511E-2</v>
       </c>
     </row>
@@ -39067,7 +39067,7 @@
         <v>0.1</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:H84" si="2">E34-$G$31*X34</f>
+        <f t="shared" ref="E35:H80" si="2">E34-$G$31*X34</f>
         <v>0.14980128794950207</v>
       </c>
       <c r="F35">
@@ -39083,7 +39083,7 @@
         <v>0.29948625112132793</v>
       </c>
       <c r="I35">
-        <f t="shared" ref="I35:I84" si="3">E35*C35+F35*D35</f>
+        <f t="shared" ref="I35:I71" si="3">E35*C35+F35*D35</f>
         <v>2.7450321987375518E-2</v>
       </c>
       <c r="J35" s="3">
@@ -39091,7 +39091,7 @@
         <v>0.50686214960490639</v>
       </c>
       <c r="K35">
-        <f t="shared" ref="K35:K84" si="5">G35*C35+H35*D35</f>
+        <f t="shared" ref="K35:K71" si="5">G35*C35+H35*D35</f>
         <v>4.2435781390165996E-2</v>
       </c>
       <c r="L35" s="7">
@@ -39099,7 +39099,7 @@
         <v>0.51060735358905995</v>
       </c>
       <c r="M35">
-        <f t="shared" ref="M35:P84" si="7">M34-$G$31*AB34</f>
+        <f t="shared" ref="M35:P80" si="7">M34-$G$31*AB34</f>
         <v>0.28525523820718612</v>
       </c>
       <c r="N35">
@@ -39115,7 +39115,7 @@
         <v>0.61735420561177679</v>
       </c>
       <c r="Q35" s="4">
-        <f t="shared" ref="Q35:Q84" si="8">M35*J35+N35*L35</f>
+        <f t="shared" ref="Q35:Q71" si="8">M35*J35+N35*L35</f>
         <v>0.31533564706720335</v>
       </c>
       <c r="R35" s="5">
@@ -39123,7 +39123,7 @@
         <v>0.57818709491369669</v>
       </c>
       <c r="S35" s="4">
-        <f t="shared" ref="S35:S84" si="10">O35*J35+P35*L35</f>
+        <f t="shared" ref="S35:S71" si="10">O35*J35+P35*L35</f>
         <v>0.60254538686637549</v>
       </c>
       <c r="T35" s="5">
@@ -39131,11 +39131,11 @@
         <v>0.64623843448737428</v>
       </c>
       <c r="U35" s="5">
-        <f t="shared" ref="U35:U84" si="12">1/2*(A35-R35)^2</f>
+        <f t="shared" ref="U35:U71" si="12">1/2*(A35-R35)^2</f>
         <v>0.16141828741323308</v>
       </c>
       <c r="V35" s="5">
-        <f t="shared" ref="V35:V84" si="13">1/2*(B35-T35)^2</f>
+        <f t="shared" ref="V35:V71" si="13">1/2*(B35-T35)^2</f>
         <v>5.9086006961845627E-2</v>
       </c>
       <c r="W35" s="5">
@@ -39143,35 +39143,35 @@
         <v>0.22050429437507871</v>
       </c>
       <c r="X35" s="4">
-        <f t="shared" ref="X35:X84" si="15">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*C35</f>
+        <f t="shared" ref="X35:X71" si="15">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*C35</f>
         <v>-6.273914906283137E-5</v>
       </c>
       <c r="Y35" s="4">
-        <f t="shared" ref="Y35:Y84" si="16">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*D35</f>
+        <f t="shared" ref="Y35:Y71" si="16">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*D35</f>
         <v>-1.2547829812566274E-4</v>
       </c>
       <c r="Z35" s="4">
-        <f t="shared" ref="Z35:Z84" si="17">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*C35</f>
+        <f t="shared" ref="Z35:Z71" si="17">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*C35</f>
         <v>-2.7203725468020798E-5</v>
       </c>
       <c r="AA35" s="4">
-        <f t="shared" ref="AA35:AA84" si="18">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*D35</f>
+        <f t="shared" ref="AA35:AA71" si="18">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*D35</f>
         <v>-5.4407450936041596E-5</v>
       </c>
       <c r="AB35" s="4">
-        <f t="shared" ref="AB35:AB84" si="19">(R35-A35)*R35*(1-R35)*J35</f>
+        <f t="shared" ref="AB35:AB71" si="19">(R35-A35)*R35*(1-R35)*J35</f>
         <v>7.0237570846521838E-2</v>
       </c>
       <c r="AC35" s="4">
-        <f t="shared" ref="AC35:AC84" si="20">(R35-A35)*R35*(1-R35)*L35</f>
+        <f t="shared" ref="AC35:AC71" si="20">(R35-A35)*R35*(1-R35)*L35</f>
         <v>7.0756556196634707E-2</v>
       </c>
       <c r="AD35">
-        <f t="shared" ref="AD35:AD84" si="21">(T35-B35)*T35*(1-T35)*J35</f>
+        <f t="shared" ref="AD35:AD71" si="21">(T35-B35)*T35*(1-T35)*J35</f>
         <v>-3.983369653584206E-2</v>
       </c>
       <c r="AE35">
-        <f t="shared" ref="AE35:AE84" si="22">(T35-B35)*T35*(1-T35)*L35</f>
+        <f t="shared" ref="AE35:AE71" si="22">(T35-B35)*T35*(1-T35)*L35</f>
         <v>-4.0128027685023125E-2</v>
       </c>
     </row>
@@ -44743,7 +44743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B7947C-67C1-4E5A-8E7D-ACE592354F5B}">
   <dimension ref="A2:AE84"/>
   <sheetViews>
-    <sheetView topLeftCell="C5" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView topLeftCell="G5" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
@@ -45293,7 +45293,7 @@
         <v>0.1</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:H84" si="2">E34-$G$31*X34</f>
+        <f t="shared" ref="E35:H80" si="2">E34-$G$31*X34</f>
         <v>0.14978312799586518</v>
       </c>
       <c r="F35">
@@ -45309,7 +45309,7 @@
         <v>0.29942111303725494</v>
       </c>
       <c r="I35">
-        <f t="shared" ref="I35:I84" si="3">E35*C35+F35*D35</f>
+        <f t="shared" ref="I35:I71" si="3">E35*C35+F35*D35</f>
         <v>2.7445781998966294E-2</v>
       </c>
       <c r="J35" s="3">
@@ -45317,7 +45317,7 @@
         <v>0.50686101482155277</v>
       </c>
       <c r="K35">
-        <f t="shared" ref="K35:K84" si="5">G35*C35+H35*D35</f>
+        <f t="shared" ref="K35:K71" si="5">G35*C35+H35*D35</f>
         <v>4.2427639129656872E-2</v>
       </c>
       <c r="L35" s="7">
@@ -45325,7 +45325,7 @@
         <v>0.51060531893989114</v>
       </c>
       <c r="M35">
-        <f t="shared" ref="M35:P84" si="7">M34-$G$31*AB34</f>
+        <f t="shared" ref="M35:P80" si="7">M34-$G$31*AB34</f>
         <v>0.25681628948610918</v>
       </c>
       <c r="N35">
@@ -45341,7 +45341,7 @@
         <v>0.63385749999789709</v>
       </c>
       <c r="Q35" s="4">
-        <f t="shared" ref="Q35:Q84" si="8">M35*J35+N35*L35</f>
+        <f t="shared" ref="Q35:Q71" si="8">M35*J35+N35*L35</f>
         <v>0.28629162862228796</v>
       </c>
       <c r="R35" s="5">
@@ -45349,7 +45349,7 @@
         <v>0.57108802080462751</v>
       </c>
       <c r="S35" s="4">
-        <f t="shared" ref="S35:S84" si="10">O35*J35+P35*L35</f>
+        <f t="shared" ref="S35:S71" si="10">O35*J35+P35*L35</f>
         <v>0.61927365319216143</v>
       </c>
       <c r="T35" s="5">
@@ -45357,11 +45357,11 @@
         <v>0.65005333431296386</v>
       </c>
       <c r="U35" s="5">
-        <f t="shared" ref="U35:U84" si="12">1/2*(A35-R35)^2</f>
+        <f t="shared" ref="U35:U71" si="12">1/2*(A35-R35)^2</f>
         <v>0.15740988354522706</v>
       </c>
       <c r="V35" s="5">
-        <f t="shared" ref="V35:V84" si="13">1/2*(B35-T35)^2</f>
+        <f t="shared" ref="V35:V71" si="13">1/2*(B35-T35)^2</f>
         <v>5.7781867755866752E-2</v>
       </c>
       <c r="W35" s="5">
@@ -45369,35 +45369,35 @@
         <v>0.2151917513010938</v>
       </c>
       <c r="X35" s="4">
-        <f t="shared" ref="X35:X84" si="15">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*C35</f>
+        <f t="shared" ref="X35:X71" si="15">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*C35</f>
         <v>-1.2257163433034129E-4</v>
       </c>
       <c r="Y35" s="4">
-        <f t="shared" ref="Y35:Y84" si="16">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*D35</f>
+        <f t="shared" ref="Y35:Y71" si="16">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*D35</f>
         <v>-2.4514326866068259E-4</v>
       </c>
       <c r="Z35" s="4">
-        <f t="shared" ref="Z35:Z84" si="17">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*C35</f>
+        <f t="shared" ref="Z35:Z71" si="17">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*C35</f>
         <v>-8.7404022399914652E-5</v>
       </c>
       <c r="AA35" s="4">
-        <f t="shared" ref="AA35:AA84" si="18">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*D35</f>
+        <f t="shared" ref="AA35:AA71" si="18">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*D35</f>
         <v>-1.748080447998293E-4</v>
       </c>
       <c r="AB35" s="4">
-        <f t="shared" ref="AB35:AB84" si="19">(R35-A35)*R35*(1-R35)*J35</f>
+        <f t="shared" ref="AB35:AB71" si="19">(R35-A35)*R35*(1-R35)*J35</f>
         <v>6.9661225723248885E-2</v>
       </c>
       <c r="AC35" s="4">
-        <f t="shared" ref="AC35:AC84" si="20">(R35-A35)*R35*(1-R35)*L35</f>
+        <f t="shared" ref="AC35:AC71" si="20">(R35-A35)*R35*(1-R35)*L35</f>
         <v>7.0175829937691961E-2</v>
       </c>
       <c r="AD35">
-        <f t="shared" ref="AD35:AD84" si="21">(T35-B35)*T35*(1-T35)*J35</f>
+        <f t="shared" ref="AD35:AD71" si="21">(T35-B35)*T35*(1-T35)*J35</f>
         <v>-3.9196792037676453E-2</v>
       </c>
       <c r="AE35">
-        <f t="shared" ref="AE35:AE84" si="22">(T35-B35)*T35*(1-T35)*L35</f>
+        <f t="shared" ref="AE35:AE71" si="22">(T35-B35)*T35*(1-T35)*L35</f>
         <v>-3.9486348159691466E-2</v>
       </c>
     </row>
@@ -50969,7 +50969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C93EEE2-1974-4649-88B6-19406246D6E1}">
   <dimension ref="A2:AE84"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H3" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
@@ -51519,7 +51519,7 @@
         <v>0.1</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:H84" si="2">E34-$G$31*X34</f>
+        <f t="shared" ref="E35:H80" si="2">E34-$G$31*X34</f>
         <v>0.14987418725180882</v>
       </c>
       <c r="F35">
@@ -51535,7 +51535,7 @@
         <v>0.29946137204959927</v>
       </c>
       <c r="I35">
-        <f t="shared" ref="I35:I84" si="3">E35*C35+F35*D35</f>
+        <f t="shared" ref="I35:I71" si="3">E35*C35+F35*D35</f>
         <v>2.7468546812952209E-2</v>
       </c>
       <c r="J35" s="3">
@@ -51543,7 +51543,7 @@
         <v>0.50686670495254016</v>
       </c>
       <c r="K35">
-        <f t="shared" ref="K35:K84" si="5">G35*C35+H35*D35</f>
+        <f t="shared" ref="K35:K71" si="5">G35*C35+H35*D35</f>
         <v>4.2432671506199914E-2</v>
       </c>
       <c r="L35" s="7">
@@ -51551,7 +51551,7 @@
         <v>0.51060657646795427</v>
       </c>
       <c r="M35">
-        <f t="shared" ref="M35:P84" si="7">M34-$G$31*AB34</f>
+        <f t="shared" ref="M35:P80" si="7">M34-$G$31*AB34</f>
         <v>0.11641378967052787</v>
       </c>
       <c r="N35">
@@ -51567,7 +51567,7 @@
         <v>0.71438017127274211</v>
       </c>
       <c r="Q35" s="4">
-        <f t="shared" ref="Q35:Q84" si="8">M35*J35+N35*L35</f>
+        <f t="shared" ref="Q35:Q71" si="8">M35*J35+N35*L35</f>
         <v>0.14290791978034093</v>
       </c>
       <c r="R35" s="5">
@@ -51575,7 +51575,7 @@
         <v>0.53566630049507913</v>
       </c>
       <c r="S35" s="4">
-        <f t="shared" ref="S35:S84" si="10">O35*J35+P35*L35</f>
+        <f t="shared" ref="S35:S71" si="10">O35*J35+P35*L35</f>
         <v>0.70090804233644399</v>
       </c>
       <c r="T35" s="5">
@@ -51583,11 +51583,11 @@
         <v>0.66838906608788662</v>
       </c>
       <c r="U35" s="5">
-        <f t="shared" ref="U35:U84" si="12">1/2*(A35-R35)^2</f>
+        <f t="shared" ref="U35:U71" si="12">1/2*(A35-R35)^2</f>
         <v>0.1381625297380914</v>
       </c>
       <c r="V35" s="5">
-        <f t="shared" ref="V35:V84" si="13">1/2*(B35-T35)^2</f>
+        <f t="shared" ref="V35:V71" si="13">1/2*(B35-T35)^2</f>
         <v>5.1716796405910877E-2</v>
       </c>
       <c r="W35" s="5">
@@ -51595,35 +51595,35 @@
         <v>0.18987932614400227</v>
       </c>
       <c r="X35" s="4">
-        <f t="shared" ref="X35:X84" si="15">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*C35</f>
+        <f t="shared" ref="X35:X71" si="15">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*C35</f>
         <v>-4.0058074685720384E-4</v>
       </c>
       <c r="Y35" s="4">
-        <f t="shared" ref="Y35:Y84" si="16">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*D35</f>
+        <f t="shared" ref="Y35:Y71" si="16">((R35-A35)*R35*(1-R35)*M35+(T35-B35)*T35*(1-T35)*O35)*J35*(1-J35)*D35</f>
         <v>-8.0116149371440768E-4</v>
       </c>
       <c r="Z35" s="4">
-        <f t="shared" ref="Z35:Z84" si="17">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*C35</f>
+        <f t="shared" ref="Z35:Z71" si="17">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*C35</f>
         <v>-3.6782612037413787E-4</v>
       </c>
       <c r="AA35" s="4">
-        <f t="shared" ref="AA35:AA84" si="18">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*D35</f>
+        <f t="shared" ref="AA35:AA71" si="18">((R35-A35)*R35*(1-R35)*N35+(T35-B35)*T35*(1-T35)*P35)*L35*(1-L35)*D35</f>
         <v>-7.3565224074827575E-4</v>
       </c>
       <c r="AB35" s="4">
-        <f t="shared" ref="AB35:AB84" si="19">(R35-A35)*R35*(1-R35)*J35</f>
+        <f t="shared" ref="AB35:AB71" si="19">(R35-A35)*R35*(1-R35)*J35</f>
         <v>6.6271748591446675E-2</v>
       </c>
       <c r="AC35" s="4">
-        <f t="shared" ref="AC35:AC84" si="20">(R35-A35)*R35*(1-R35)*L35</f>
+        <f t="shared" ref="AC35:AC71" si="20">(R35-A35)*R35*(1-R35)*L35</f>
         <v>6.6760728874452335E-2</v>
       </c>
       <c r="AD35">
-        <f t="shared" ref="AD35:AD84" si="21">(T35-B35)*T35*(1-T35)*J35</f>
+        <f t="shared" ref="AD35:AD71" si="21">(T35-B35)*T35*(1-T35)*J35</f>
         <v>-3.6131230136519511E-2</v>
       </c>
       <c r="AE35">
-        <f t="shared" ref="AE35:AE84" si="22">(T35-B35)*T35*(1-T35)*L35</f>
+        <f t="shared" ref="AE35:AE71" si="22">(T35-B35)*T35*(1-T35)*L35</f>
         <v>-3.6397821248313075E-2</v>
       </c>
     </row>

</xml_diff>